<commit_message>
20210816 2232 tlw87 file updates for today.
</commit_message>
<xml_diff>
--- a/docs/ERS_Testing.xlsx
+++ b/docs/ERS_Testing.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw8748253\Desktop\Projects\ProjectShell\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw87\Desktop\Projects\Expense-Reimbursement-System\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA23F1E-460C-46FD-B120-DAE093EB33BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15530" activeTab="1"/>
+    <workbookView xWindow="645" yWindow="5850" windowWidth="27465" windowHeight="8550" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
   <si>
     <t>Test Class</t>
   </si>
@@ -78,19 +79,58 @@
     <t>Parameters / Body</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>GeneralServiceTest</t>
   </si>
   <si>
-    <t>http://localhost:3015/general</t>
-  </si>
-  <si>
-    <t>/general</t>
-  </si>
-  <si>
-    <t>All records returned.</t>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>testGetAllRecords_EmptyDataBase</t>
+  </si>
+  <si>
+    <t>GeneralService</t>
+  </si>
+  <si>
+    <t>getAllRecords</t>
+  </si>
+  <si>
+    <t>Exception test case when no records are in the database</t>
+  </si>
+  <si>
+    <t>testGetAllRecords_Success</t>
+  </si>
+  <si>
+    <t>Success test case return all mock records defined</t>
+  </si>
+  <si>
+    <t>Post Man</t>
+  </si>
+  <si>
+    <t>/ers_login</t>
+  </si>
+  <si>
+    <t>http://localhost:3015/ers_login</t>
+  </si>
+  <si>
+    <t>?username=tlw874&amp;password=123456</t>
+  </si>
+  <si>
+    <t>Get login request: VALID password.</t>
+  </si>
+  <si>
+    <t>Validated User</t>
+  </si>
+  <si>
+    <t>Get login request: INVALID password</t>
+  </si>
+  <si>
+    <t>?username=tlw874&amp;password=12345678</t>
+  </si>
+  <si>
+    <t>User not validated</t>
   </si>
   <si>
     <r>
@@ -112,112 +152,14 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>"General was not found in the database."</t>
-    </r>
-  </si>
-  <si>
-    <t>Expected</t>
-  </si>
-  <si>
-    <t>no records returned</t>
-  </si>
-  <si>
-    <t>all records return</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Prior to initial data load</t>
-  </si>
-  <si>
-    <t>After initial data load</t>
-  </si>
-  <si>
-    <t>Get general request All Records: Records Returned</t>
-  </si>
-  <si>
-    <t>Get general request All Records: No records return</t>
-  </si>
-  <si>
-    <t>Get general request All Records: Bad Request</t>
-  </si>
-  <si>
-    <t>Get general request All Records: Wrong Port</t>
-  </si>
-  <si>
-    <t>http://localhost:3015/genera</t>
-  </si>
-  <si>
-    <t>Not Found</t>
-  </si>
-  <si>
-    <t>connection refused</t>
-  </si>
-  <si>
-    <t>Error: connect ECONNREFUSED 127.0.0.1:3010</t>
-  </si>
-  <si>
-    <t>http://localhost:3010/general</t>
-  </si>
-  <si>
-    <t>testGetAllRecords_EmptyDataBase</t>
-  </si>
-  <si>
-    <t>GeneralService</t>
-  </si>
-  <si>
-    <t>getAllRecords</t>
-  </si>
-  <si>
-    <t>Exception test case when no records are in the database</t>
-  </si>
-  <si>
-    <t>testGetAllRecords_Success</t>
-  </si>
-  <si>
-    <t>Success test case return all mock records defined</t>
-  </si>
-  <si>
-    <t>Post Man</t>
-  </si>
-  <si>
-    <t>Get general request All Records: No database error</t>
-  </si>
-  <si>
-    <t>Table not created</t>
-  </si>
-  <si>
-    <t>database error caught</t>
-  </si>
-  <si>
-    <r>
-      <t>"message"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF0451A5"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"Error with database getting all General records."</t>
+      <t>"Autentication failed for username and password provided."</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000.00"/>
   </numFmts>
@@ -339,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -402,9 +344,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -693,7 +632,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -701,18 +640,18 @@
       <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="26"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,47 +670,47 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G1" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="26">
+        <v>23</v>
+      </c>
+      <c r="G2" s="25">
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="26">
+        <v>25</v>
+      </c>
+      <c r="G3" s="25">
         <v>0.02</v>
       </c>
     </row>
@@ -782,31 +721,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="57.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="4"/>
+    <col min="4" max="4" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -826,16 +765,16 @@
         <v>16</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>0</v>
       </c>
@@ -843,89 +782,67 @@
         <v>9</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>46</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="G2" s="18"/>
       <c r="H2" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>27</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G3" s="18"/>
       <c r="H3" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="10">
-        <v>0.02</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10">
-        <v>5</v>
-      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
@@ -937,65 +854,33 @@
       <c r="H5" s="18"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="10">
-        <v>0.03</v>
-      </c>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="10">
-        <v>0.04</v>
-      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="23"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1010,7 +895,7 @@
       <c r="H8" s="18"/>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>10</v>
       </c>
@@ -1025,7 +910,7 @@
       <c r="H9" s="18"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>10.01</v>
       </c>
@@ -1040,7 +925,7 @@
       <c r="H10" s="18"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10.02</v>
       </c>
@@ -1055,7 +940,7 @@
       <c r="H11" s="18"/>
       <c r="I11" s="21"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>10.029999999999999</v>
       </c>
@@ -1070,7 +955,7 @@
       <c r="H12" s="18"/>
       <c r="I12" s="21"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>15</v>
       </c>
@@ -1085,7 +970,7 @@
       <c r="H13" s="18"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>15.01</v>
       </c>
@@ -1100,7 +985,7 @@
       <c r="H14" s="18"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>15.02</v>
       </c>
@@ -1115,7 +1000,7 @@
       <c r="H15" s="18"/>
       <c r="I15" s="21"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15.03</v>
       </c>
@@ -1130,7 +1015,7 @@
       <c r="H16" s="18"/>
       <c r="I16" s="21"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>20</v>
       </c>
@@ -1145,7 +1030,7 @@
       <c r="H17" s="18"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>20.010000000000002</v>
       </c>
@@ -1160,7 +1045,7 @@
       <c r="H18" s="18"/>
       <c r="I18" s="22"/>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>20.02</v>
       </c>
@@ -1175,7 +1060,7 @@
       <c r="H19" s="18"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>21</v>
       </c>
@@ -1190,7 +1075,7 @@
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>21.01</v>
       </c>
@@ -1205,7 +1090,7 @@
       <c r="H21" s="18"/>
       <c r="I21" s="21"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21.02</v>
       </c>
@@ -1220,7 +1105,7 @@
       <c r="H22" s="18"/>
       <c r="I22" s="21"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>25</v>
       </c>
@@ -1235,7 +1120,7 @@
       <c r="H23" s="18"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>25.01</v>
       </c>
@@ -1250,7 +1135,7 @@
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>25.02</v>
       </c>
@@ -1265,7 +1150,7 @@
       <c r="H25" s="18"/>
       <c r="I25" s="21"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>25.03</v>
       </c>
@@ -1280,7 +1165,7 @@
       <c r="H26" s="18"/>
       <c r="I26" s="21"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>25.04</v>
       </c>
@@ -1295,7 +1180,7 @@
       <c r="H27" s="18"/>
       <c r="I27" s="21"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>0</v>
       </c>
@@ -1310,7 +1195,7 @@
       <c r="H28" s="18"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>0.01</v>
       </c>
@@ -1325,7 +1210,7 @@
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>0.02</v>
       </c>
@@ -1340,7 +1225,7 @@
       <c r="H30" s="18"/>
       <c r="I30" s="21"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>0.03</v>
       </c>
@@ -1355,7 +1240,7 @@
       <c r="H31" s="18"/>
       <c r="I31" s="21"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>1</v>
       </c>
@@ -1370,7 +1255,7 @@
       <c r="H32" s="18"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <v>2</v>
       </c>
@@ -1385,7 +1270,7 @@
       <c r="H33" s="18"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>5</v>
       </c>
@@ -1400,7 +1285,7 @@
       <c r="H34" s="18"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
         <v>6</v>
       </c>
@@ -1415,7 +1300,7 @@
       <c r="H35" s="18"/>
       <c r="I35" s="18"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>0</v>
       </c>
@@ -1430,7 +1315,7 @@
       <c r="H36" s="18"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
         <v>5</v>
       </c>
@@ -1445,7 +1330,7 @@
       <c r="H37" s="18"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>5.01</v>
       </c>
@@ -1460,7 +1345,7 @@
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>0</v>
       </c>
@@ -1475,7 +1360,7 @@
       <c r="H39" s="18"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>0</v>
       </c>
@@ -1490,7 +1375,7 @@
       <c r="H40" s="18"/>
       <c r="I40" s="18"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>5</v>
       </c>
@@ -1505,7 +1390,7 @@
       <c r="H41" s="18"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>5</v>
       </c>
@@ -1520,7 +1405,7 @@
       <c r="H42" s="18"/>
       <c r="I42" s="18"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>5.01</v>
       </c>
@@ -1535,7 +1420,7 @@
       <c r="H43" s="18"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="13"/>
       <c r="C44" s="12"/>
@@ -1546,7 +1431,7 @@
       <c r="H44" s="12"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="13"/>
       <c r="C45" s="12"/>
@@ -1557,7 +1442,7 @@
       <c r="H45" s="12"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="13"/>
       <c r="C46" s="12"/>
@@ -1568,7 +1453,7 @@
       <c r="H46" s="12"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="13"/>
       <c r="C47" s="12"/>
@@ -1579,7 +1464,7 @@
       <c r="H47" s="12"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="13"/>
       <c r="C48" s="12"/>
@@ -1590,7 +1475,7 @@
       <c r="H48" s="12"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="13"/>
       <c r="C49" s="12"/>
@@ -1601,7 +1486,7 @@
       <c r="H49" s="12"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="13"/>
       <c r="C50" s="12"/>
@@ -1612,7 +1497,7 @@
       <c r="H50" s="12"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="13"/>
       <c r="C51" s="12"/>
@@ -1623,7 +1508,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="13"/>
       <c r="C52" s="12"/>
@@ -1634,7 +1519,7 @@
       <c r="H52" s="12"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="13"/>
       <c r="C53" s="12"/>
@@ -1645,7 +1530,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="13"/>
       <c r="C54" s="12"/>
@@ -1656,7 +1541,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="13"/>
       <c r="C55" s="12"/>
@@ -1667,7 +1552,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="13"/>
       <c r="C56" s="12"/>
@@ -1678,7 +1563,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="13"/>
       <c r="C57" s="12"/>
@@ -1689,7 +1574,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="13"/>
       <c r="C58" s="12"/>
@@ -1700,7 +1585,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="13"/>
       <c r="C59" s="12"/>
@@ -1711,7 +1596,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="13"/>
       <c r="C60" s="12"/>
@@ -1722,7 +1607,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
@@ -1733,7 +1618,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
@@ -1744,7 +1629,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
@@ -1755,7 +1640,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
@@ -1766,7 +1651,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
@@ -1777,7 +1662,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>

</xml_diff>

<commit_message>
20210818 1720 tlw8748253: file updates for today.
</commit_message>
<xml_diff>
--- a/docs/ERS_Testing.xlsx
+++ b/docs/ERS_Testing.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw87\Desktop\Projects\Expense-Reimbursement-System\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw8748253\Desktop\Projects\Expense-Reimbursement-System\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA23F1E-460C-46FD-B120-DAE093EB33BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="5850" windowWidth="27465" windowHeight="8550" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="650" yWindow="5850" windowWidth="27470" windowHeight="8550"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
   <si>
     <t>Test Class</t>
   </si>
@@ -79,31 +78,10 @@
     <t>Parameters / Body</t>
   </si>
   <si>
-    <t>GeneralServiceTest</t>
-  </si>
-  <si>
     <t>Expected</t>
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>testGetAllRecords_EmptyDataBase</t>
-  </si>
-  <si>
-    <t>GeneralService</t>
-  </si>
-  <si>
-    <t>getAllRecords</t>
-  </si>
-  <si>
-    <t>Exception test case when no records are in the database</t>
-  </si>
-  <si>
-    <t>testGetAllRecords_Success</t>
-  </si>
-  <si>
-    <t>Success test case return all mock records defined</t>
   </si>
   <si>
     <t>Post Man</t>
@@ -155,13 +133,80 @@
       <t>"Autentication failed for username and password provided."</t>
     </r>
   </si>
+  <si>
+    <t>ERSAdminServiceTest</t>
+  </si>
+  <si>
+    <t>ERSAdminService</t>
+  </si>
+  <si>
+    <t>addReimbursementStatus</t>
+  </si>
+  <si>
+    <t>Success added new Reimbursement status to database.</t>
+  </si>
+  <si>
+    <t>Expected: Exception adding duplicate Reimbursement status to database.</t>
+  </si>
+  <si>
+    <t>testAddReimbursementStatusDuplicate</t>
+  </si>
+  <si>
+    <t>testAddReimbursementStatusSuccess</t>
+  </si>
+  <si>
+    <t>testAddReimbursementStatusBadParamStatus</t>
+  </si>
+  <si>
+    <t>testAddReimbursementStatusBadParamStatusDesc</t>
+  </si>
+  <si>
+    <t>Expected: Exception adding bad parameter. Status less than 6.</t>
+  </si>
+  <si>
+    <t>Expected: Exception adding bad parameter. No Status Description.</t>
+  </si>
+  <si>
+    <t>testAddReimbursementTypeSuccess</t>
+  </si>
+  <si>
+    <t>testGetAllReimbursementStatusSuccess</t>
+  </si>
+  <si>
+    <t>testGetAllReimbursementStatusException</t>
+  </si>
+  <si>
+    <t>getAllReimbursementStatus</t>
+  </si>
+  <si>
+    <t>Success get all reimbursement statuses from the database.</t>
+  </si>
+  <si>
+    <t>Expected: Exception getting records from the database.</t>
+  </si>
+  <si>
+    <t>testGetAllReimbursementTypeSuccess</t>
+  </si>
+  <si>
+    <t>addReimbursementType</t>
+  </si>
+  <si>
+    <t>Success added new Reimbursement type to database.</t>
+  </si>
+  <si>
+    <t>getAllReimbursementType</t>
+  </si>
+  <si>
+    <t>Success get all reimbursement types from the database.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="000.00"/>
+    <numFmt numFmtId="165" formatCode="00.000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -281,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -353,6 +398,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,30 +679,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="25"/>
+    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -671,47 +718,125 @@
         <v>4</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2">
+        <v>29</v>
+      </c>
+      <c r="B2" s="28">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="25">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B3" s="28">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B4" s="28">
+        <v>1.002</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="28">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="28">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="25">
-        <v>0.02</v>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B7" s="28">
+        <v>2.0009999999999999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B8" s="28">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B9" s="28">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -721,31 +846,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="5" customWidth="1"/>
     <col min="4" max="4" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="5" max="5" width="29.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -765,16 +890,16 @@
         <v>16</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>0</v>
       </c>
@@ -782,26 +907,26 @@
         <v>9</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="18" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -809,26 +934,26 @@
         <v>9</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
         <v>9</v>
@@ -841,7 +966,7 @@
       <c r="H4" s="18"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
         <v>9</v>
@@ -854,7 +979,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
         <v>9</v>
@@ -867,7 +992,7 @@
       <c r="H6" s="18"/>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
         <v>9</v>
@@ -880,7 +1005,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="23"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -895,7 +1020,7 @@
       <c r="H8" s="18"/>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
         <v>10</v>
       </c>
@@ -910,7 +1035,7 @@
       <c r="H9" s="18"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
         <v>10.01</v>
       </c>
@@ -925,7 +1050,7 @@
       <c r="H10" s="18"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>10.02</v>
       </c>
@@ -940,7 +1065,7 @@
       <c r="H11" s="18"/>
       <c r="I11" s="21"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>10.029999999999999</v>
       </c>
@@ -955,7 +1080,7 @@
       <c r="H12" s="18"/>
       <c r="I12" s="21"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
         <v>15</v>
       </c>
@@ -970,7 +1095,7 @@
       <c r="H13" s="18"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>15.01</v>
       </c>
@@ -985,7 +1110,7 @@
       <c r="H14" s="18"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
         <v>15.02</v>
       </c>
@@ -1000,7 +1125,7 @@
       <c r="H15" s="18"/>
       <c r="I15" s="21"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
         <v>15.03</v>
       </c>
@@ -1015,7 +1140,7 @@
       <c r="H16" s="18"/>
       <c r="I16" s="21"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>20</v>
       </c>
@@ -1030,7 +1155,7 @@
       <c r="H17" s="18"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
         <v>20.010000000000002</v>
       </c>
@@ -1045,7 +1170,7 @@
       <c r="H18" s="18"/>
       <c r="I18" s="22"/>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
         <v>20.02</v>
       </c>
@@ -1060,7 +1185,7 @@
       <c r="H19" s="18"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
         <v>21</v>
       </c>
@@ -1075,7 +1200,7 @@
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <v>21.01</v>
       </c>
@@ -1090,7 +1215,7 @@
       <c r="H21" s="18"/>
       <c r="I21" s="21"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
         <v>21.02</v>
       </c>
@@ -1105,7 +1230,7 @@
       <c r="H22" s="18"/>
       <c r="I22" s="21"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
         <v>25</v>
       </c>
@@ -1120,7 +1245,7 @@
       <c r="H23" s="18"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
         <v>25.01</v>
       </c>
@@ -1135,7 +1260,7 @@
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="10">
         <v>25.02</v>
       </c>
@@ -1150,7 +1275,7 @@
       <c r="H25" s="18"/>
       <c r="I25" s="21"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
         <v>25.03</v>
       </c>
@@ -1165,7 +1290,7 @@
       <c r="H26" s="18"/>
       <c r="I26" s="21"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
         <v>25.04</v>
       </c>
@@ -1180,7 +1305,7 @@
       <c r="H27" s="18"/>
       <c r="I27" s="21"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
         <v>0</v>
       </c>
@@ -1195,7 +1320,7 @@
       <c r="H28" s="18"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="14">
         <v>0.01</v>
       </c>
@@ -1210,7 +1335,7 @@
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="14">
         <v>0.02</v>
       </c>
@@ -1225,7 +1350,7 @@
       <c r="H30" s="18"/>
       <c r="I30" s="21"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="14">
         <v>0.03</v>
       </c>
@@ -1240,7 +1365,7 @@
       <c r="H31" s="18"/>
       <c r="I31" s="21"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="14">
         <v>1</v>
       </c>
@@ -1255,7 +1380,7 @@
       <c r="H32" s="18"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="14">
         <v>2</v>
       </c>
@@ -1270,7 +1395,7 @@
       <c r="H33" s="18"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="14">
         <v>5</v>
       </c>
@@ -1285,7 +1410,7 @@
       <c r="H34" s="18"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="14">
         <v>6</v>
       </c>
@@ -1300,7 +1425,7 @@
       <c r="H35" s="18"/>
       <c r="I35" s="18"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="14">
         <v>0</v>
       </c>
@@ -1315,7 +1440,7 @@
       <c r="H36" s="18"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="14">
         <v>5</v>
       </c>
@@ -1330,7 +1455,7 @@
       <c r="H37" s="18"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="10">
         <v>5.01</v>
       </c>
@@ -1345,7 +1470,7 @@
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="10">
         <v>0</v>
       </c>
@@ -1360,7 +1485,7 @@
       <c r="H39" s="18"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="10">
         <v>0</v>
       </c>
@@ -1375,7 +1500,7 @@
       <c r="H40" s="18"/>
       <c r="I40" s="18"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="10">
         <v>5</v>
       </c>
@@ -1390,7 +1515,7 @@
       <c r="H41" s="18"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="10">
         <v>5</v>
       </c>
@@ -1405,7 +1530,7 @@
       <c r="H42" s="18"/>
       <c r="I42" s="18"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="10">
         <v>5.01</v>
       </c>
@@ -1420,7 +1545,7 @@
       <c r="H43" s="18"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="10"/>
       <c r="B44" s="13"/>
       <c r="C44" s="12"/>
@@ -1431,7 +1556,7 @@
       <c r="H44" s="12"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="10"/>
       <c r="B45" s="13"/>
       <c r="C45" s="12"/>
@@ -1442,7 +1567,7 @@
       <c r="H45" s="12"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="10"/>
       <c r="B46" s="13"/>
       <c r="C46" s="12"/>
@@ -1453,7 +1578,7 @@
       <c r="H46" s="12"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="10"/>
       <c r="B47" s="13"/>
       <c r="C47" s="12"/>
@@ -1464,7 +1589,7 @@
       <c r="H47" s="12"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="10"/>
       <c r="B48" s="13"/>
       <c r="C48" s="12"/>
@@ -1475,7 +1600,7 @@
       <c r="H48" s="12"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="10"/>
       <c r="B49" s="13"/>
       <c r="C49" s="12"/>
@@ -1486,7 +1611,7 @@
       <c r="H49" s="12"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="10"/>
       <c r="B50" s="13"/>
       <c r="C50" s="12"/>
@@ -1497,7 +1622,7 @@
       <c r="H50" s="12"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="10"/>
       <c r="B51" s="13"/>
       <c r="C51" s="12"/>
@@ -1508,7 +1633,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="10"/>
       <c r="B52" s="13"/>
       <c r="C52" s="12"/>
@@ -1519,7 +1644,7 @@
       <c r="H52" s="12"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="10"/>
       <c r="B53" s="13"/>
       <c r="C53" s="12"/>
@@ -1530,7 +1655,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="10"/>
       <c r="B54" s="13"/>
       <c r="C54" s="12"/>
@@ -1541,7 +1666,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="10"/>
       <c r="B55" s="13"/>
       <c r="C55" s="12"/>
@@ -1552,7 +1677,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="10"/>
       <c r="B56" s="13"/>
       <c r="C56" s="12"/>
@@ -1563,7 +1688,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="10"/>
       <c r="B57" s="13"/>
       <c r="C57" s="12"/>
@@ -1574,7 +1699,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="10"/>
       <c r="B58" s="13"/>
       <c r="C58" s="12"/>
@@ -1585,7 +1710,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="10"/>
       <c r="B59" s="13"/>
       <c r="C59" s="12"/>
@@ -1596,7 +1721,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="10"/>
       <c r="B60" s="13"/>
       <c r="C60" s="12"/>
@@ -1607,7 +1732,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="10"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
@@ -1618,7 +1743,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="10"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
@@ -1629,7 +1754,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="10"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
@@ -1640,7 +1765,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="10"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
@@ -1651,7 +1776,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="10"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
@@ -1662,7 +1787,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="10"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>

</xml_diff>

<commit_message>
20210818 2339 tlw87 file updates for today.
</commit_message>
<xml_diff>
--- a/docs/ERS_Testing.xlsx
+++ b/docs/ERS_Testing.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw8748253\Desktop\Projects\Expense-Reimbursement-System\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw87\Desktop\Projects\Expense-Reimbursement-System\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6AC793-BF13-40E8-985B-8017D82A777C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="650" yWindow="5850" windowWidth="27470" windowHeight="8550"/>
+    <workbookView xWindow="645" yWindow="5850" windowWidth="27465" windowHeight="8550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t>Test Class</t>
   </si>
@@ -199,11 +200,29 @@
   <si>
     <t>Success get all reimbursement types from the database.</t>
   </si>
+  <si>
+    <t>testAddUserRoleSuccess</t>
+  </si>
+  <si>
+    <t>addUserRole</t>
+  </si>
+  <si>
+    <t>Success added new User Role to database.</t>
+  </si>
+  <si>
+    <t>testGetAllUserRoleSuccess</t>
+  </si>
+  <si>
+    <t>getAllRecords</t>
+  </si>
+  <si>
+    <t>Success get all user roles from the database.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="000.00"/>
     <numFmt numFmtId="165" formatCode="00.000"/>
@@ -679,26 +698,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="25"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -721,7 +740,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -741,7 +760,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="28">
         <v>1.0009999999999999</v>
       </c>
@@ -755,7 +774,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="28">
         <v>1.002</v>
       </c>
@@ -769,7 +788,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="28">
         <v>1.0029999999999999</v>
       </c>
@@ -783,7 +802,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="28">
         <v>2</v>
       </c>
@@ -797,7 +816,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="28">
         <v>2.0009999999999999</v>
       </c>
@@ -811,7 +830,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="28">
         <v>3</v>
       </c>
@@ -825,7 +844,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="28">
         <v>4</v>
       </c>
@@ -837,6 +856,34 @@
       </c>
       <c r="F9" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="28">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="28">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -846,7 +893,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -856,21 +903,21 @@
       <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="5" customWidth="1"/>
     <col min="4" max="4" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="4"/>
+    <col min="5" max="5" width="29.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -899,7 +946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>0</v>
       </c>
@@ -926,7 +973,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -953,7 +1000,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
         <v>9</v>
@@ -966,7 +1013,7 @@
       <c r="H4" s="18"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
         <v>9</v>
@@ -979,7 +1026,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
         <v>9</v>
@@ -992,7 +1039,7 @@
       <c r="H6" s="18"/>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
         <v>9</v>
@@ -1005,7 +1052,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="23"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1020,7 +1067,7 @@
       <c r="H8" s="18"/>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>10</v>
       </c>
@@ -1035,7 +1082,7 @@
       <c r="H9" s="18"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>10.01</v>
       </c>
@@ -1050,7 +1097,7 @@
       <c r="H10" s="18"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10.02</v>
       </c>
@@ -1065,7 +1112,7 @@
       <c r="H11" s="18"/>
       <c r="I11" s="21"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>10.029999999999999</v>
       </c>
@@ -1080,7 +1127,7 @@
       <c r="H12" s="18"/>
       <c r="I12" s="21"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>15</v>
       </c>
@@ -1095,7 +1142,7 @@
       <c r="H13" s="18"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>15.01</v>
       </c>
@@ -1110,7 +1157,7 @@
       <c r="H14" s="18"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>15.02</v>
       </c>
@@ -1125,7 +1172,7 @@
       <c r="H15" s="18"/>
       <c r="I15" s="21"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15.03</v>
       </c>
@@ -1140,7 +1187,7 @@
       <c r="H16" s="18"/>
       <c r="I16" s="21"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>20</v>
       </c>
@@ -1155,7 +1202,7 @@
       <c r="H17" s="18"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>20.010000000000002</v>
       </c>
@@ -1170,7 +1217,7 @@
       <c r="H18" s="18"/>
       <c r="I18" s="22"/>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>20.02</v>
       </c>
@@ -1185,7 +1232,7 @@
       <c r="H19" s="18"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>21</v>
       </c>
@@ -1200,7 +1247,7 @@
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>21.01</v>
       </c>
@@ -1215,7 +1262,7 @@
       <c r="H21" s="18"/>
       <c r="I21" s="21"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21.02</v>
       </c>
@@ -1230,7 +1277,7 @@
       <c r="H22" s="18"/>
       <c r="I22" s="21"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>25</v>
       </c>
@@ -1245,7 +1292,7 @@
       <c r="H23" s="18"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>25.01</v>
       </c>
@@ -1260,7 +1307,7 @@
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>25.02</v>
       </c>
@@ -1275,7 +1322,7 @@
       <c r="H25" s="18"/>
       <c r="I25" s="21"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>25.03</v>
       </c>
@@ -1290,7 +1337,7 @@
       <c r="H26" s="18"/>
       <c r="I26" s="21"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>25.04</v>
       </c>
@@ -1305,7 +1352,7 @@
       <c r="H27" s="18"/>
       <c r="I27" s="21"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>0</v>
       </c>
@@ -1320,7 +1367,7 @@
       <c r="H28" s="18"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>0.01</v>
       </c>
@@ -1335,7 +1382,7 @@
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>0.02</v>
       </c>
@@ -1350,7 +1397,7 @@
       <c r="H30" s="18"/>
       <c r="I30" s="21"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>0.03</v>
       </c>
@@ -1365,7 +1412,7 @@
       <c r="H31" s="18"/>
       <c r="I31" s="21"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>1</v>
       </c>
@@ -1380,7 +1427,7 @@
       <c r="H32" s="18"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <v>2</v>
       </c>
@@ -1395,7 +1442,7 @@
       <c r="H33" s="18"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>5</v>
       </c>
@@ -1410,7 +1457,7 @@
       <c r="H34" s="18"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
         <v>6</v>
       </c>
@@ -1425,7 +1472,7 @@
       <c r="H35" s="18"/>
       <c r="I35" s="18"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>0</v>
       </c>
@@ -1440,7 +1487,7 @@
       <c r="H36" s="18"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
         <v>5</v>
       </c>
@@ -1455,7 +1502,7 @@
       <c r="H37" s="18"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>5.01</v>
       </c>
@@ -1470,7 +1517,7 @@
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>0</v>
       </c>
@@ -1485,7 +1532,7 @@
       <c r="H39" s="18"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>0</v>
       </c>
@@ -1500,7 +1547,7 @@
       <c r="H40" s="18"/>
       <c r="I40" s="18"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>5</v>
       </c>
@@ -1515,7 +1562,7 @@
       <c r="H41" s="18"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>5</v>
       </c>
@@ -1530,7 +1577,7 @@
       <c r="H42" s="18"/>
       <c r="I42" s="18"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>5.01</v>
       </c>
@@ -1545,7 +1592,7 @@
       <c r="H43" s="18"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="13"/>
       <c r="C44" s="12"/>
@@ -1556,7 +1603,7 @@
       <c r="H44" s="12"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="13"/>
       <c r="C45" s="12"/>
@@ -1567,7 +1614,7 @@
       <c r="H45" s="12"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="13"/>
       <c r="C46" s="12"/>
@@ -1578,7 +1625,7 @@
       <c r="H46" s="12"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="13"/>
       <c r="C47" s="12"/>
@@ -1589,7 +1636,7 @@
       <c r="H47" s="12"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="13"/>
       <c r="C48" s="12"/>
@@ -1600,7 +1647,7 @@
       <c r="H48" s="12"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="13"/>
       <c r="C49" s="12"/>
@@ -1611,7 +1658,7 @@
       <c r="H49" s="12"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="13"/>
       <c r="C50" s="12"/>
@@ -1622,7 +1669,7 @@
       <c r="H50" s="12"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="13"/>
       <c r="C51" s="12"/>
@@ -1633,7 +1680,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="13"/>
       <c r="C52" s="12"/>
@@ -1644,7 +1691,7 @@
       <c r="H52" s="12"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="13"/>
       <c r="C53" s="12"/>
@@ -1655,7 +1702,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="13"/>
       <c r="C54" s="12"/>
@@ -1666,7 +1713,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="13"/>
       <c r="C55" s="12"/>
@@ -1677,7 +1724,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="13"/>
       <c r="C56" s="12"/>
@@ -1688,7 +1735,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="13"/>
       <c r="C57" s="12"/>
@@ -1699,7 +1746,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="13"/>
       <c r="C58" s="12"/>
@@ -1710,7 +1757,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="13"/>
       <c r="C59" s="12"/>
@@ -1721,7 +1768,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="13"/>
       <c r="C60" s="12"/>
@@ -1732,7 +1779,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
@@ -1743,7 +1790,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
@@ -1754,7 +1801,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
@@ -1765,7 +1812,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
@@ -1776,7 +1823,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
@@ -1787,7 +1834,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>

</xml_diff>

<commit_message>
20210819 2210 tlw87 file updates for today.
</commit_message>
<xml_diff>
--- a/docs/ERS_Testing.xlsx
+++ b/docs/ERS_Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw87\Desktop\Projects\Expense-Reimbursement-System\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6AC793-BF13-40E8-985B-8017D82A777C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC050C1-A566-43DB-8F47-90A93B0BBC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="5850" windowWidth="27465" windowHeight="8550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="465" yWindow="5070" windowWidth="27465" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
   <si>
     <t>Test Class</t>
   </si>
@@ -218,6 +218,27 @@
   <si>
     <t>Success get all user roles from the database.</t>
   </si>
+  <si>
+    <t>ERSService</t>
+  </si>
+  <si>
+    <t>test_addNewUserSuccess</t>
+  </si>
+  <si>
+    <t>ERSServiceTest</t>
+  </si>
+  <si>
+    <t>addNewUser</t>
+  </si>
+  <si>
+    <t>Success adding a user.</t>
+  </si>
+  <si>
+    <t>test_addNewUserBadPwdNoCapLetter</t>
+  </si>
+  <si>
+    <t>Expected: BadParameterException.  Logfile: password eror contains no capital letter.</t>
+  </si>
 </sst>
 </file>
 
@@ -225,7 +246,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="000.00"/>
-    <numFmt numFmtId="165" formatCode="00.000"/>
+    <numFmt numFmtId="166" formatCode="000.000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -417,8 +438,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,11 +720,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +734,7 @@
     <col min="3" max="3" width="47.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" style="25"/>
   </cols>
   <sheetData>
@@ -761,12 +782,18 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
       <c r="B3" s="28">
         <v>1.0009999999999999</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
       </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
       <c r="E3" t="s">
         <v>31</v>
       </c>
@@ -775,12 +802,18 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
       <c r="B4" s="28">
         <v>1.002</v>
       </c>
       <c r="C4" t="s">
         <v>36</v>
       </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
       <c r="E4" t="s">
         <v>31</v>
       </c>
@@ -789,12 +822,18 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
       <c r="B5" s="28">
         <v>1.0029999999999999</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
       </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
       <c r="E5" t="s">
         <v>31</v>
       </c>
@@ -803,12 +842,18 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
       <c r="B6" s="28">
         <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>41</v>
       </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
       <c r="E6" t="s">
         <v>43</v>
       </c>
@@ -817,12 +862,18 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
       <c r="B7" s="28">
         <v>2.0009999999999999</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
       </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
       <c r="E7" t="s">
         <v>43</v>
       </c>
@@ -831,12 +882,18 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
       <c r="B8" s="28">
         <v>3</v>
       </c>
       <c r="C8" t="s">
         <v>40</v>
       </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
       <c r="E8" t="s">
         <v>47</v>
       </c>
@@ -845,12 +902,18 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
       <c r="B9" s="28">
         <v>4</v>
       </c>
       <c r="C9" t="s">
         <v>46</v>
       </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
       <c r="E9" t="s">
         <v>49</v>
       </c>
@@ -859,12 +922,18 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
       <c r="B10" s="28">
         <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>51</v>
       </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
       <c r="E10" t="s">
         <v>52</v>
       </c>
@@ -873,17 +942,57 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
       <c r="B11" s="28">
         <v>6</v>
       </c>
       <c r="C11" t="s">
         <v>54</v>
       </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
       <c r="E11" t="s">
         <v>55</v>
       </c>
       <c r="F11" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="28">
+        <v>100</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="28">
+        <v>101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20210826 2019 tlw87 checkpoint [corrected null object].
</commit_message>
<xml_diff>
--- a/docs/ERS_Testing.xlsx
+++ b/docs/ERS_Testing.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw87\Desktop\Projects\Expense-Reimbursement-System\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC050C1-A566-43DB-8F47-90A93B0BBC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC7F21D-30ED-48BB-B076-8304D33CE056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="5070" windowWidth="27465" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="465" yWindow="5070" windowWidth="27465" windowHeight="9990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit" sheetId="1" r:id="rId1"/>
     <sheet name="Postman" sheetId="2" r:id="rId2"/>
+    <sheet name="RTM" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="107">
   <si>
     <t>Test Class</t>
   </si>
@@ -239,6 +240,135 @@
   <si>
     <t>Expected: BadParameterException.  Logfile: password eror contains no capital letter.</t>
   </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>All employees in the company can login</t>
+  </si>
+  <si>
+    <t>All employees can submit requests for reimbursement</t>
+  </si>
+  <si>
+    <t>All employees can view their past tickets</t>
+  </si>
+  <si>
+    <t>Role 1</t>
+  </si>
+  <si>
+    <t>Role 2</t>
+  </si>
+  <si>
+    <t>EMPLOYEE</t>
+  </si>
+  <si>
+    <t>FINANCEMGR</t>
+  </si>
+  <si>
+    <t>All employees can view their pending requests</t>
+  </si>
+  <si>
+    <t>Finance managers can log in</t>
+  </si>
+  <si>
+    <t>Finance managers can view all reimbursement requests</t>
+  </si>
+  <si>
+    <t>Finance managers can view past history for all employees in the company</t>
+  </si>
+  <si>
+    <t>Finance managers are authorized to approve requests for expense reimbursement</t>
+  </si>
+  <si>
+    <t>Finance managers are authorized to deny requests for expense reimbursement</t>
+  </si>
+  <si>
+    <t>Role 3</t>
+  </si>
+  <si>
+    <t>Role 4</t>
+  </si>
+  <si>
+    <t>Timestamps provide history.</t>
+  </si>
+  <si>
+    <t>Reimbursement request status when created is PENDING</t>
+  </si>
+  <si>
+    <t>BACKEND</t>
+  </si>
+  <si>
+    <t>Reimbursement request final state APPROVED cannot be changed</t>
+  </si>
+  <si>
+    <t>FRONT-END</t>
+  </si>
+  <si>
+    <t>Reimbursement request final state DENIED cannot be changed</t>
+  </si>
+  <si>
+    <t>Employees can select reimbursement type of  LODGING</t>
+  </si>
+  <si>
+    <t>Employees can select reimbursement type of  TRAVEL</t>
+  </si>
+  <si>
+    <t>Employees can select reimbursement type of  FOOD,</t>
+  </si>
+  <si>
+    <t>Employees can select reimbursement type of  OTHER.</t>
+  </si>
+  <si>
+    <t>Only allowable reimbursement types are LODGING, TRAVEL, FOOD, or OTHER</t>
+  </si>
+  <si>
+    <t>UC Financial Manager ==&gt; login</t>
+  </si>
+  <si>
+    <t>Use Case Employee</t>
+  </si>
+  <si>
+    <t>Use Case Financial Manager</t>
+  </si>
+  <si>
+    <t>UC  ==&gt; login</t>
+  </si>
+  <si>
+    <t>UC  ==&gt; Add reimbursement request</t>
+  </si>
+  <si>
+    <t>UC for FM should generalize from Employee</t>
+  </si>
+  <si>
+    <t>UC ==&gt; View past tickets</t>
+  </si>
+  <si>
+    <t>As Employee</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>UC ==&gt; View all reimbursements for all employees</t>
+  </si>
+  <si>
+    <t>Implied</t>
+  </si>
+  <si>
+    <t>UC ==&gt; Approve/deny reimbursement</t>
+  </si>
+  <si>
+    <t>No written requirement</t>
+  </si>
+  <si>
+    <t>UC ==&gt; Filter view request by status</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
 </sst>
 </file>
 
@@ -246,7 +376,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="000.00"/>
-    <numFmt numFmtId="166" formatCode="000.000"/>
+    <numFmt numFmtId="165" formatCode="000.000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -307,7 +437,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,6 +465,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -438,8 +574,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,7 +873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
@@ -1958,4 +2109,436 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C77A310-F525-46D4-AFD9-DE5E739D29B1}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" style="29" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" style="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="34"/>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" s="34"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="34"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="34"/>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="34"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="32"/>
+      <c r="D8" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" s="34"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" s="34"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="32"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="32"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="32"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="32"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="32"/>
+      <c r="F16" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="32"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="32"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="32"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="32"/>
+      <c r="H19" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="I19" s="34"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>